<commit_message>
Update 4-key word list
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pairs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="330">
   <si>
     <t>er</t>
   </si>
@@ -1001,6 +1002,9 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>dvorak</t>
   </si>
 </sst>
 </file>
@@ -1770,11 +1774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="71397888"/>
-        <c:axId val="47412864"/>
+        <c:axId val="107378688"/>
+        <c:axId val="98357760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71397888"/>
+        <c:axId val="107378688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,7 +1787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47412864"/>
+        <c:crossAx val="98357760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1791,7 +1795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47412864"/>
+        <c:axId val="98357760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,14 +1806,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71397888"/>
+        <c:crossAx val="107378688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2148,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5174,4 +5177,1738 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1">
+        <v>301.8</v>
+      </c>
+      <c r="C1">
+        <v>3.8</v>
+      </c>
+      <c r="E1">
+        <f>B1-B2</f>
+        <v>120.5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1">
+        <v>1078</v>
+      </c>
+      <c r="L1" s="1">
+        <f>K1/$K$25</f>
+        <v>0.13824057450628366</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="O1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P1" t="s">
+        <v>320</v>
+      </c>
+      <c r="S1" t="s">
+        <v>329</v>
+      </c>
+      <c r="T1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2">
+        <v>181.3</v>
+      </c>
+      <c r="C2">
+        <v>1.9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K2">
+        <v>867</v>
+      </c>
+      <c r="L2" s="1">
+        <f>K2/$K$25</f>
+        <v>0.11118235444985894</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="O2">
+        <v>181.3</v>
+      </c>
+      <c r="P2">
+        <v>301.8</v>
+      </c>
+      <c r="Q2">
+        <f>P2-O2</f>
+        <v>120.5</v>
+      </c>
+      <c r="S2">
+        <v>1.9</v>
+      </c>
+      <c r="T2">
+        <v>3.8</v>
+      </c>
+      <c r="U2">
+        <f>T2-S2</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3">
+        <v>275.89999999999998</v>
+      </c>
+      <c r="C3">
+        <v>3.8</v>
+      </c>
+      <c r="E3" s="1">
+        <f>($B$1-B3)/$E$1</f>
+        <v>0.21493775933609988</v>
+      </c>
+      <c r="F3" s="1">
+        <f>($B$1-B3)/$E$1</f>
+        <v>0.21493775933609988</v>
+      </c>
+      <c r="J3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K3">
+        <v>696</v>
+      </c>
+      <c r="L3" s="1">
+        <f>K3/$K$25</f>
+        <v>8.9253654783277764E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>281</v>
+      </c>
+      <c r="O3">
+        <v>180.1</v>
+      </c>
+      <c r="P3">
+        <v>261.39999999999998</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>((P$2-P3)-(O$2-O3))/Q$2</f>
+        <v>0.3253112033195022</v>
+      </c>
+      <c r="R3" s="1">
+        <f>Q3-L1</f>
+        <v>0.18707062881321854</v>
+      </c>
+      <c r="S3">
+        <v>1.8</v>
+      </c>
+      <c r="T3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U3" s="1">
+        <f>((T$2-T3)-(S$2-S3))/U$2/2</f>
+        <v>0.36842105263157898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4">
+        <v>241.7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <f>($B$1-B4)/$E$1</f>
+        <v>0.49875518672199187</v>
+      </c>
+      <c r="F4" s="2">
+        <f>E4-E3</f>
+        <v>0.283817427385892</v>
+      </c>
+      <c r="J4" t="s">
+        <v>290</v>
+      </c>
+      <c r="K4">
+        <v>592</v>
+      </c>
+      <c r="L4" s="1">
+        <f>K4/$K$25</f>
+        <v>7.5916901769684533E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>282</v>
+      </c>
+      <c r="O4">
+        <v>180.5</v>
+      </c>
+      <c r="P4">
+        <v>262.5</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>((P$2-P4)-(O$2-O4))/Q$2</f>
+        <v>0.31950207468879666</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R26" si="0">Q4-L2</f>
+        <v>0.20831972023893772</v>
+      </c>
+      <c r="S4">
+        <v>1.8</v>
+      </c>
+      <c r="T4">
+        <v>3.4</v>
+      </c>
+      <c r="U4" s="1">
+        <f t="shared" ref="U4:U26" si="1">((T$2-T4)-(S$2-S4))/U$2/2</f>
+        <v>7.8947368421052641E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5">
+        <v>235.4</v>
+      </c>
+      <c r="C5">
+        <v>5.5</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E26" si="2">($B$1-B5)/$E$1</f>
+        <v>0.55103734439834029</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F26" si="3">E5-E4</f>
+        <v>5.2282157676348417E-2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5">
+        <v>561</v>
+      </c>
+      <c r="L5" s="1">
+        <f>K5/$K$25</f>
+        <v>7.1941523467555779E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>283</v>
+      </c>
+      <c r="O5">
+        <v>180.5</v>
+      </c>
+      <c r="P5">
+        <v>275.8</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>((P$2-P5)-(O$2-O5))/Q$2</f>
+        <v>0.20912863070539409</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11987497592211632</v>
+      </c>
+      <c r="S5">
+        <v>1.9</v>
+      </c>
+      <c r="T5">
+        <v>3.4</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10526315789473682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6">
+        <v>234.8</v>
+      </c>
+      <c r="C6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.55601659751037347</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9792531120331773E-3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>286</v>
+      </c>
+      <c r="K6">
+        <v>558</v>
+      </c>
+      <c r="L6" s="1">
+        <f>K6/$K$25</f>
+        <v>7.155680943831752E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>290</v>
+      </c>
+      <c r="O6">
+        <v>181</v>
+      </c>
+      <c r="P6">
+        <v>278.89999999999998</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>((P$2-P6)-(O$2-O6))/Q$2</f>
+        <v>0.18755186721991721</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11163496545023267</v>
+      </c>
+      <c r="S6">
+        <v>1.6</v>
+      </c>
+      <c r="T6">
+        <v>3.7</v>
+      </c>
+      <c r="U6" s="1">
+        <f>((T$2-T6)-(S$2-S6))/U$2/2</f>
+        <v>-5.2631578947368474E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B7">
+        <v>226.1</v>
+      </c>
+      <c r="C7">
+        <v>5.2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.62821576763485487</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2199170124481404E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>287</v>
+      </c>
+      <c r="K7">
+        <v>506</v>
+      </c>
+      <c r="L7" s="1">
+        <f>K7/$K$25</f>
+        <v>6.4888432931520898E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>284</v>
+      </c>
+      <c r="O7">
+        <v>156.9</v>
+      </c>
+      <c r="P7">
+        <v>277.5</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" ref="Q7:Q26" si="4">((P$2-P7)-(O$2-O7))/Q$2</f>
+        <v>-8.2987551867215199E-4</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.2771398986227934E-2</v>
+      </c>
+      <c r="S7">
+        <v>1.5</v>
+      </c>
+      <c r="T7">
+        <v>3.6</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.2631578947368474E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8">
+        <v>208.3</v>
+      </c>
+      <c r="C8">
+        <v>5.2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.77593360995850624</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.14771784232365137</v>
+      </c>
+      <c r="J8" t="s">
+        <v>288</v>
+      </c>
+      <c r="K8">
+        <v>453</v>
+      </c>
+      <c r="L8" s="1">
+        <f>K8/$K$25</f>
+        <v>5.8091818414978201E-2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>286</v>
+      </c>
+      <c r="O8">
+        <v>180.8</v>
+      </c>
+      <c r="P8">
+        <v>278.5</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="4"/>
+        <v>0.18921161825726152</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.117654808818944</v>
+      </c>
+      <c r="S8">
+        <v>1.8</v>
+      </c>
+      <c r="T8">
+        <v>3.5</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="1"/>
+        <v>5.2631578947368411E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9">
+        <v>209.6</v>
+      </c>
+      <c r="C9">
+        <v>4.8</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.7651452282157678</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.078838174273844E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>289</v>
+      </c>
+      <c r="K9">
+        <v>418</v>
+      </c>
+      <c r="L9" s="1">
+        <f>K9/$K$25</f>
+        <v>5.3603488073865092E-2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>287</v>
+      </c>
+      <c r="O9">
+        <v>180.7</v>
+      </c>
+      <c r="P9">
+        <v>301.39999999999998</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.659751037344304E-3</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.6548183968865207E-2</v>
+      </c>
+      <c r="S9">
+        <v>1.8</v>
+      </c>
+      <c r="T9">
+        <v>3.7</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.8432790769745078E-17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B10">
+        <v>208.9</v>
+      </c>
+      <c r="C10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.77095435684647307</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>5.8091286307052625E-3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>291</v>
+      </c>
+      <c r="K10">
+        <v>387</v>
+      </c>
+      <c r="L10" s="1">
+        <f>K10/$K$25</f>
+        <v>4.9628109771736345E-2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>288</v>
+      </c>
+      <c r="O10">
+        <v>163</v>
+      </c>
+      <c r="P10">
+        <v>284.5</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="4"/>
+        <v>-8.2987551867219917E-3</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.6390573601700198E-2</v>
+      </c>
+      <c r="S10">
+        <v>1.8</v>
+      </c>
+      <c r="T10">
+        <v>3.3</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10526315789473688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11">
+        <v>186.8</v>
+      </c>
+      <c r="C11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.9543568464730291</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18340248962655603</v>
+      </c>
+      <c r="J11" t="s">
+        <v>296</v>
+      </c>
+      <c r="K11">
+        <v>252</v>
+      </c>
+      <c r="L11" s="1">
+        <f>K11/$K$25</f>
+        <v>3.231597845601436E-2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>289</v>
+      </c>
+      <c r="O11">
+        <v>167.4</v>
+      </c>
+      <c r="P11">
+        <v>301.5</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.11286307053941903</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.16646655861328413</v>
+      </c>
+      <c r="S11">
+        <v>1.8</v>
+      </c>
+      <c r="T11">
+        <v>3.4</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8947368421052641E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B12">
+        <v>185.9</v>
+      </c>
+      <c r="C12">
+        <v>3.7</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.96182572614107886</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="3"/>
+        <v>7.468879668049766E-3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>292</v>
+      </c>
+      <c r="K12">
+        <v>249</v>
+      </c>
+      <c r="L12" s="1">
+        <f>K12/$K$25</f>
+        <v>3.1931264426776095E-2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>291</v>
+      </c>
+      <c r="O12">
+        <v>166.1</v>
+      </c>
+      <c r="P12">
+        <v>300.8</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.11784232365145242</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.16747043342318876</v>
+      </c>
+      <c r="S12">
+        <v>1.8</v>
+      </c>
+      <c r="T12">
+        <v>2.7</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26315789473684204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B13">
+        <v>183.3</v>
+      </c>
+      <c r="C13">
+        <v>3.2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98340248962655596</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1576763485477102E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>299</v>
+      </c>
+      <c r="K13">
+        <v>202</v>
+      </c>
+      <c r="L13" s="1">
+        <f>K13/$K$25</f>
+        <v>2.5904077968709926E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>296</v>
+      </c>
+      <c r="O13">
+        <v>169.6</v>
+      </c>
+      <c r="P13">
+        <v>290.89999999999998</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>((P$2-P13)-(O$2-O13))/Q$2</f>
+        <v>-6.6390041493774518E-3</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.8954982605391812E-2</v>
+      </c>
+      <c r="S13">
+        <v>1.8</v>
+      </c>
+      <c r="T13">
+        <v>3.7</v>
+      </c>
+      <c r="U13" s="1">
+        <f>((T$2-T13)-(S$2-S13))/U$2/2</f>
+        <v>-5.8432790769745078E-17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B14">
+        <v>183.5</v>
+      </c>
+      <c r="C14">
+        <v>3.1</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98174273858921168</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.6597510373442814E-3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>297</v>
+      </c>
+      <c r="K14">
+        <v>186</v>
+      </c>
+      <c r="L14" s="1">
+        <f>K14/$K$25</f>
+        <v>2.3852269812772504E-2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>292</v>
+      </c>
+      <c r="O14">
+        <v>181.2</v>
+      </c>
+      <c r="P14">
+        <v>292.2</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="4"/>
+        <v>7.8838174273858919E-2</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6906909847082824E-2</v>
+      </c>
+      <c r="S14">
+        <v>1.7</v>
+      </c>
+      <c r="T14">
+        <v>3.3</v>
+      </c>
+      <c r="U14" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8947368421052641E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15">
+        <v>182.8</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98755186721991706</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="3"/>
+        <v>5.8091286307053736E-3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>294</v>
+      </c>
+      <c r="K15">
+        <v>171</v>
+      </c>
+      <c r="L15" s="1">
+        <f>K15/$K$25</f>
+        <v>2.1928699666581175E-2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>299</v>
+      </c>
+      <c r="O15">
+        <v>173.4</v>
+      </c>
+      <c r="P15">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>((P$2-P15)-(O$2-O15))/Q$2</f>
+        <v>-1.6597510373445399E-3</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.7563829006054467E-2</v>
+      </c>
+      <c r="S15">
+        <v>1.6</v>
+      </c>
+      <c r="T15">
+        <v>3.7</v>
+      </c>
+      <c r="U15" s="1">
+        <f>((T$2-T15)-(S$2-S15))/U$2/2</f>
+        <v>-5.2631578947368474E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16">
+        <v>182.9</v>
+      </c>
+      <c r="C16">
+        <v>2.1</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98672199170124486</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="3"/>
+        <v>-8.2987551867219622E-4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>295</v>
+      </c>
+      <c r="K16">
+        <v>163</v>
+      </c>
+      <c r="L16" s="1">
+        <f>K16/$K$25</f>
+        <v>2.0902795588612466E-2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>297</v>
+      </c>
+      <c r="O16">
+        <v>170.1</v>
+      </c>
+      <c r="P16">
+        <v>301.39999999999998</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>((P$2-P16)-(O$2-O16))/Q$2</f>
+        <v>-8.9626556016597372E-2</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.11347882582936988</v>
+      </c>
+      <c r="S16">
+        <v>1.9</v>
+      </c>
+      <c r="T16">
+        <v>3.7</v>
+      </c>
+      <c r="U16" s="1">
+        <f>((T$2-T16)-(S$2-S16))/U$2/2</f>
+        <v>2.6315789473684119E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17">
+        <v>184.7</v>
+      </c>
+      <c r="C17">
+        <v>2.1</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.97178423236514544</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.4937759336099421E-2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>300</v>
+      </c>
+      <c r="K17">
+        <v>141</v>
+      </c>
+      <c r="L17" s="1">
+        <f>K17/$K$25</f>
+        <v>1.8081559374198513E-2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>294</v>
+      </c>
+      <c r="O17">
+        <v>174.5</v>
+      </c>
+      <c r="P17">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="4"/>
+        <v>7.4688796680496038E-3</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4459819998531572E-2</v>
+      </c>
+      <c r="S17">
+        <v>1.8</v>
+      </c>
+      <c r="T17">
+        <v>3.3</v>
+      </c>
+      <c r="U17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10526315789473688</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18">
+        <v>183.8</v>
+      </c>
+      <c r="C18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.97925311203319498</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="3"/>
+        <v>7.468879668049544E-3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>298</v>
+      </c>
+      <c r="K18">
+        <v>131</v>
+      </c>
+      <c r="L18" s="1">
+        <f>K18/$K$25</f>
+        <v>1.6799179276737627E-2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>295</v>
+      </c>
+      <c r="O18">
+        <v>173.6</v>
+      </c>
+      <c r="P18">
+        <v>291.8</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="4"/>
+        <v>1.908713692946044E-2</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.8156586591520259E-3</v>
+      </c>
+      <c r="S18">
+        <v>1.8</v>
+      </c>
+      <c r="T18">
+        <v>3.6</v>
+      </c>
+      <c r="U18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684178E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B19">
+        <v>183.3</v>
+      </c>
+      <c r="C19">
+        <v>2.7</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98340248962655596</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="3"/>
+        <v>4.1493775933609811E-3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>301</v>
+      </c>
+      <c r="K19">
+        <v>96</v>
+      </c>
+      <c r="L19" s="1">
+        <f>K19/$K$25</f>
+        <v>1.231084893562452E-2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>300</v>
+      </c>
+      <c r="O19">
+        <v>175.8</v>
+      </c>
+      <c r="P19">
+        <v>292.39999999999998</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="4"/>
+        <v>3.2365145228216048E-2</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4283585854017535E-2</v>
+      </c>
+      <c r="S19">
+        <v>1.8</v>
+      </c>
+      <c r="T19">
+        <v>3.7</v>
+      </c>
+      <c r="U19" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.8432790769745078E-17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20">
+        <v>181.7</v>
+      </c>
+      <c r="C20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99668049792531144</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3278008298755473E-2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>302</v>
+      </c>
+      <c r="K20">
+        <v>68</v>
+      </c>
+      <c r="L20" s="1">
+        <f>K20/$K$25</f>
+        <v>8.7201846627340349E-3</v>
+      </c>
+      <c r="N20" t="s">
+        <v>298</v>
+      </c>
+      <c r="O20">
+        <v>176.7</v>
+      </c>
+      <c r="P20">
+        <v>297.10000000000002</v>
+      </c>
+      <c r="Q20" s="1">
+        <f>((P$2-P20)-(O$2-O20))/Q$2</f>
+        <v>8.2987551867191617E-4</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5969303758065712E-2</v>
+      </c>
+      <c r="S20">
+        <v>1.6</v>
+      </c>
+      <c r="T20">
+        <v>3.7</v>
+      </c>
+      <c r="U20" s="1">
+        <f>((T$2-T20)-(S$2-S20))/U$2/2</f>
+        <v>-5.2631578947368474E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>301</v>
+      </c>
+      <c r="B21">
+        <v>181.4</v>
+      </c>
+      <c r="C21">
+        <v>2.7</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.9991701244813278</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="3"/>
+        <v>2.4896265560163666E-3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>303</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21" s="1">
+        <f>K21/$K$25</f>
+        <v>8.9766606822262122E-4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>301</v>
+      </c>
+      <c r="O21">
+        <v>177.4</v>
+      </c>
+      <c r="P21">
+        <v>301.7</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.1535269709543429E-2</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.384611864516795E-2</v>
+      </c>
+      <c r="S21">
+        <v>1.8</v>
+      </c>
+      <c r="T21">
+        <v>3.6</v>
+      </c>
+      <c r="U21" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684178E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>302</v>
+      </c>
+      <c r="B22">
+        <v>181.8</v>
+      </c>
+      <c r="C22">
+        <v>2.1</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99585062240663902</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.3195020746887849E-3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>304</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22" s="1">
+        <f>K22/$K$25</f>
+        <v>7.6942805847653249E-4</v>
+      </c>
+      <c r="N22" t="s">
+        <v>302</v>
+      </c>
+      <c r="O22">
+        <v>178.1</v>
+      </c>
+      <c r="P22">
+        <v>299</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="4"/>
+        <v>-3.3195020746888439E-3</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.2039686737422879E-2</v>
+      </c>
+      <c r="S22">
+        <v>1.9</v>
+      </c>
+      <c r="T22">
+        <v>3.8</v>
+      </c>
+      <c r="U22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>303</v>
+      </c>
+      <c r="B23">
+        <v>181</v>
+      </c>
+      <c r="C23">
+        <v>2.1</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0024896265560166</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="3"/>
+        <v>6.6390041493775698E-3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>306</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23" s="1">
+        <f>K23/$K$25</f>
+        <v>7.6942805847653249E-4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>303</v>
+      </c>
+      <c r="O23">
+        <v>180.9</v>
+      </c>
+      <c r="P23">
+        <v>301.5</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="4"/>
+        <v>-8.2987551867215199E-4</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.7275415868947732E-3</v>
+      </c>
+      <c r="S23">
+        <v>1.9</v>
+      </c>
+      <c r="T23">
+        <v>3.8</v>
+      </c>
+      <c r="U23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B24">
+        <v>180.9</v>
+      </c>
+      <c r="C24">
+        <v>2.1</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0033195020746888</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="3"/>
+        <v>8.2987551867219622E-4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>305</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24" s="1">
+        <f>K24/$K$25</f>
+        <v>5.1295203898435492E-4</v>
+      </c>
+      <c r="N24" t="s">
+        <v>304</v>
+      </c>
+      <c r="O24">
+        <v>181</v>
+      </c>
+      <c r="P24">
+        <v>301.8</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.4896265560166919E-3</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.2590546144932245E-3</v>
+      </c>
+      <c r="S24">
+        <v>1.9</v>
+      </c>
+      <c r="T24">
+        <v>3.7</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6315789473684119E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>305</v>
+      </c>
+      <c r="B25">
+        <v>181.3</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.3195020746887849E-3</v>
+      </c>
+      <c r="K25">
+        <f>SUM(K1:K24)</f>
+        <v>7798</v>
+      </c>
+      <c r="L25" s="2">
+        <f>SUM(L1:L24)</f>
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>306</v>
+      </c>
+      <c r="O25">
+        <v>181</v>
+      </c>
+      <c r="P25">
+        <v>301.60000000000002</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>((P$2-P25)-(O$2-O25))/Q$2</f>
+        <v>-8.2987551867238791E-4</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5993035771489205E-3</v>
+      </c>
+      <c r="S25">
+        <v>1.9</v>
+      </c>
+      <c r="T25">
+        <v>3.8</v>
+      </c>
+      <c r="U25" s="1">
+        <f>((T$2-T25)-(S$2-S25))/U$2/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B26">
+        <v>181.1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0016597510373446</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6597510373446145E-3</v>
+      </c>
+      <c r="N26" t="s">
+        <v>305</v>
+      </c>
+      <c r="O26">
+        <v>181.1</v>
+      </c>
+      <c r="P26">
+        <v>301.5</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="4"/>
+        <v>8.2987551867215199E-4</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1692347968779707E-4</v>
+      </c>
+      <c r="S26">
+        <v>1.9</v>
+      </c>
+      <c r="T26">
+        <v>3.8</v>
+      </c>
+      <c r="U26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q27" s="2">
+        <f>SUM(Q3:Q26)</f>
+        <v>0.99170124481327782</v>
+      </c>
+      <c r="R27" s="2">
+        <f>SUM(R3:R26)</f>
+        <v>-8.2987551867221409E-3</v>
+      </c>
+      <c r="U27" s="2">
+        <f>SUM(U3:U26)</f>
+        <v>1.1315789473684199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <f>SUM(H33:H43)</f>
+        <v>1.3701244813278011</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>281</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.3253112033195022</v>
+      </c>
+      <c r="I33" s="2">
+        <f>H33/I$32</f>
+        <v>0.23743185947910361</v>
+      </c>
+      <c r="J33" s="2">
+        <f>SUM(I$33:I33)</f>
+        <v>0.23743185947910361</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>282</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.31950207468879666</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" ref="I34:I43" si="5">H34/I$32</f>
+        <v>0.23319200484554808</v>
+      </c>
+      <c r="J34" s="2">
+        <f>SUM(I$33:I34)</f>
+        <v>0.4706238643246517</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>283</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.20912863070539409</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="5"/>
+        <v>0.15263476680799506</v>
+      </c>
+      <c r="J35" s="2">
+        <f>SUM(I$33:I35)</f>
+        <v>0.62325863113264679</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>286</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.18921161825726152</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="5"/>
+        <v>0.13809812235009092</v>
+      </c>
+      <c r="J36" s="2">
+        <f>SUM(I$33:I36)</f>
+        <v>0.76135675348273768</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>290</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.18755186721991721</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="5"/>
+        <v>0.13688673531193227</v>
+      </c>
+      <c r="J37" s="2">
+        <f>SUM(I$33:I37)</f>
+        <v>0.89824348879466998</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>292</v>
+      </c>
+      <c r="H38" s="1">
+        <v>7.8838174273858919E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="5"/>
+        <v>5.7540884312537843E-2</v>
+      </c>
+      <c r="J38" s="2">
+        <f>SUM(I$33:I38)</f>
+        <v>0.95578437310720776</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>300</v>
+      </c>
+      <c r="H39" s="1">
+        <v>3.2365145228216048E-2</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3622047244094689E-2</v>
+      </c>
+      <c r="J39" s="2">
+        <f>SUM(I$33:I39)</f>
+        <v>0.97940642035130243</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>295</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1.908713692946044E-2</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3930950938824849E-2</v>
+      </c>
+      <c r="J40" s="2">
+        <f>SUM(I$33:I40)</f>
+        <v>0.99333737129012722</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>294</v>
+      </c>
+      <c r="H41" s="1">
+        <v>7.4688796680496038E-3</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="5"/>
+        <v>5.4512416717139743E-3</v>
+      </c>
+      <c r="J41" s="2">
+        <f>SUM(I$33:I41)</f>
+        <v>0.99878861296184118</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>305</v>
+      </c>
+      <c r="H42" s="1">
+        <v>8.2987551867215199E-4</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="5"/>
+        <v>6.0569351907931136E-4</v>
+      </c>
+      <c r="J42" s="2">
+        <f>SUM(I$33:I42)</f>
+        <v>0.99939430648092054</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>298</v>
+      </c>
+      <c r="H43" s="1">
+        <v>8.2987551867191617E-4</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="5"/>
+        <v>6.0569351907913919E-4</v>
+      </c>
+      <c r="J43" s="2">
+        <f>SUM(I$33:I43)</f>
+        <v>0.99999999999999967</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>284</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-8.2987551867215199E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>303</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-8.2987551867215199E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>306</v>
+      </c>
+      <c r="H46" s="1">
+        <v>-8.2987551867238791E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>287</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-1.659751037344304E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>299</v>
+      </c>
+      <c r="H48" s="1">
+        <v>-1.6597510373445399E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>304</v>
+      </c>
+      <c r="H49" s="1">
+        <v>-2.4896265560166919E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>302</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-3.3195020746888439E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>296</v>
+      </c>
+      <c r="H51" s="1">
+        <v>-6.6390041493774518E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>288</v>
+      </c>
+      <c r="H52" s="1">
+        <v>-8.2987551867219917E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>301</v>
+      </c>
+      <c r="H53" s="1">
+        <v>-3.1535269709543429E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>297</v>
+      </c>
+      <c r="H54" s="1">
+        <v>-8.9626556016597372E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>289</v>
+      </c>
+      <c r="H55" s="1">
+        <v>-0.11286307053941903</v>
+      </c>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>291</v>
+      </c>
+      <c r="H56" s="1">
+        <v>-0.11784232365145242</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="G33:H56">
+    <sortCondition descending="1" ref="H33:H56"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>